<commit_message>
Update: Updated old implementation performance results to make them comparable to the new results (array size = 1 mil and threads count = powers of 2)
</commit_message>
<xml_diff>
--- a/Performance_Results/PerformanceResults_Consolidated.xlsx
+++ b/Performance_Results/PerformanceResults_Consolidated.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hassan.Muhammad\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E21685E7-D313-4E20-8F73-80FDE5FD9678}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DFF652-94F2-4B89-891A-42A18F1BD442}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,7 +30,7 @@
     <t>Execution Time for Multi-threaded Parallel Search</t>
   </si>
   <si>
-    <t>(Array Size: 1 billion)</t>
+    <t>(Array Size: 100 million)</t>
   </si>
   <si>
     <t># of threads</t>
@@ -40,135 +45,30 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Liberation Sans"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFCC0000"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000EE"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Liberation Sans"/>
+      <name val="Arial"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF808080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFCC0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -176,67 +76,89 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="18">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="18">
-    <cellStyle name="Accent" xfId="7"/>
-    <cellStyle name="Accent 1" xfId="8"/>
-    <cellStyle name="Accent 2" xfId="9"/>
-    <cellStyle name="Accent 3" xfId="10"/>
-    <cellStyle name="Bad" xfId="4" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Error" xfId="11"/>
-    <cellStyle name="Footnote" xfId="12"/>
-    <cellStyle name="Good" xfId="3" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading" xfId="13"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="14"/>
-    <cellStyle name="Neutral" xfId="5" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="6" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="15"/>
-    <cellStyle name="Text" xfId="16"/>
-    <cellStyle name="Warning" xfId="17"/>
+  <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000EE"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFD320"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF420E"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -287,7 +209,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> time for Multi-threaded Parallel Search</a:t>
+              <a:t> Time for Multi-threaded Parallel Search</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -295,10 +217,10 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1200" b="0" i="1" baseline="0"/>
-              <a:t>(Array Size: 1 Billion)</a:t>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>(Array Size: 100 million)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" sz="1200" b="0" i="1"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -339,7 +261,7 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -354,7 +276,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent5"/>
+              <a:schemeClr val="accent1"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -421,10 +343,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$16</c:f>
+              <c:f>Sheet1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -432,103 +354,109 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>250</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>500</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2500</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5000</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10000</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25000</c:v>
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$16</c:f>
+              <c:f>Sheet1!$B$3:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>10.87</c:v>
+                  <c:v>1.07</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.84</c:v>
+                  <c:v>1.1599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.07</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.22</c:v>
+                  <c:v>1.26</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.64</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.17</c:v>
+                  <c:v>1.1599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11.76</c:v>
+                  <c:v>1.28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.77</c:v>
+                  <c:v>1.18</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.76</c:v>
+                  <c:v>1.19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.12</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11.74</c:v>
+                  <c:v>1.28</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.42</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.19</c:v>
+                  <c:v>1.18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.75</c:v>
+                  <c:v>1.1200000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-110B-42ED-88B4-B9386C8DBEB1}"/>
+              <c16:uniqueId val="{00000000-3A3A-46FA-8DDD-4ED6E1FF9165}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -543,7 +471,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent4"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -610,10 +538,10 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$16</c:f>
+              <c:f>Sheet1!$A$3:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -621,98 +549,104 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>100</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>250</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>500</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1000</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2500</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5000</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10000</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>25000</c:v>
+                  <c:v>8192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$16</c:f>
+              <c:f>Sheet1!$C$3:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5.63</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.7</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.76</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.48</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.64</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.18</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.15</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.21</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.21</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.79</c:v>
+                  <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.44</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.01</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.35</c:v>
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-110B-42ED-88B4-B9386C8DBEB1}"/>
+              <c16:uniqueId val="{00000001-3A3A-46FA-8DDD-4ED6E1FF9165}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -727,11 +661,11 @@
         </c:dLbls>
         <c:gapWidth val="444"/>
         <c:overlap val="-90"/>
-        <c:axId val="1989711487"/>
-        <c:axId val="1995669887"/>
+        <c:axId val="1671335520"/>
+        <c:axId val="1713952144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1989711487"/>
+        <c:axId val="1671335520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,7 +710,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Threads</a:t>
+                  <a:t> of threads</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -848,7 +782,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1995669887"/>
+        <c:crossAx val="1713952144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -856,7 +790,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1995669887"/>
+        <c:axId val="1713952144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -887,7 +821,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Time (seconds)</a:t>
+                  <a:t> time (seconds)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -926,7 +860,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1989711487"/>
+        <c:crossAx val="1671335520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1014,10 +948,13 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1579,22 +1516,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>3810</xdr:colOff>
+      <xdr:colOff>64770</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>289560</xdr:colOff>
+      <xdr:colOff>518160</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF4C9A36-E8F5-4364-AC2A-E86E707EBE89}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{197EAB5D-1EEE-4E4A-97EE-41262B258814}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1616,12 +1553,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:C16" totalsRowShown="0">
-  <autoFilter ref="A2:C16"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:C16" totalsRowShown="0">
+  <autoFilter ref="A2:C16" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="# of threads"/>
-    <tableColumn id="2" name="Problem formation time (seconds)"/>
-    <tableColumn id="3" name="Thread execution time (seconds)"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="# of threads"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Problem formation time (seconds)"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Thread execution time (seconds)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1923,22 +1860,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.09765625" customWidth="1"/>
     <col min="2" max="2" width="29.296875" customWidth="1"/>
     <col min="3" max="3" width="28.69921875" customWidth="1"/>
     <col min="4" max="5" width="10.69921875" customWidth="1"/>
+    <col min="6" max="1025" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1946,173 +1884,185 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>10.87</v>
+        <v>1.07</v>
       </c>
       <c r="C3">
-        <v>5.63</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>11.84</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C4">
-        <v>5.7</v>
+        <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>12.07</v>
+        <v>1.25</v>
       </c>
       <c r="C5">
-        <v>2.76</v>
+        <v>0.32</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>12.22</v>
+        <v>1.26</v>
       </c>
       <c r="C6">
-        <v>1.48</v>
+        <v>0.19</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B7">
-        <v>11.64</v>
+        <v>1.22</v>
       </c>
       <c r="C7">
-        <v>0.64</v>
+        <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="B8">
-        <v>12.17</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="C8">
-        <v>0.32</v>
+        <v>0.09</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="B9">
-        <v>11.76</v>
+        <v>1.28</v>
       </c>
       <c r="C9">
-        <v>0.18</v>
+        <v>0.04</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>250</v>
+        <v>128</v>
       </c>
       <c r="B10">
-        <v>11.77</v>
+        <v>1.18</v>
       </c>
       <c r="C10">
-        <v>0.15</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>500</v>
+        <v>256</v>
       </c>
       <c r="B11">
-        <v>11.76</v>
+        <v>1.19</v>
       </c>
       <c r="C11">
-        <v>0.21</v>
+        <v>0.13</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1000</v>
+        <v>512</v>
       </c>
       <c r="B12">
-        <v>12.12</v>
+        <v>1.25</v>
       </c>
       <c r="C12">
-        <v>0.21</v>
+        <v>0.31</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2500</v>
+        <v>1024</v>
       </c>
       <c r="B13">
-        <v>11.74</v>
+        <v>1.28</v>
       </c>
       <c r="C13">
-        <v>0.79</v>
+        <v>0.41</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5000</v>
+        <v>2048</v>
       </c>
       <c r="B14">
-        <v>11.42</v>
+        <v>1.21</v>
       </c>
       <c r="C14">
-        <v>3.44</v>
+        <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>10000</v>
+        <v>4096</v>
       </c>
       <c r="B15">
-        <v>12.19</v>
+        <v>1.18</v>
       </c>
       <c r="C15">
-        <v>4.01</v>
+        <v>0.51</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>25000</v>
+        <v>8192</v>
       </c>
       <c r="B16">
-        <v>11.75</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="C16">
-        <v>5.35</v>
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16384</v>
+      </c>
+      <c r="B17">
+        <v>1.19</v>
+      </c>
+      <c r="C17">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39374999999999999" bottom="0.39374999999999999" header="0" footer="0"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>